<commit_message>
updated analysis files and results
</commit_message>
<xml_diff>
--- a/incentives/state_specific_data.xlsx
+++ b/incentives/state_specific_data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daltonstewart/Dropbox/Stewart-Guest_Shared/Code/Biorefinery-Tax-Incentives/incentives/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{722DD9E7-64BA-2C4D-8A4D-E95683973BE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5C925D7-9CA1-EA48-876E-EA773A86CE8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15800" xr2:uid="{ACA89B21-CD83-0545-80CD-93A328B5FE1A}"/>
   </bookViews>
@@ -18,27 +18,27 @@
   </sheets>
   <definedNames>
     <definedName name="_xlchart.v1.0" hidden="1">Sheet1!$A$2:$A$51</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">Sheet1!$L$1</definedName>
-    <definedName name="_xlchart.v1.10" hidden="1">Sheet1!$B$70:$B$119</definedName>
-    <definedName name="_xlchart.v1.11" hidden="1">Sheet1!$C$69</definedName>
-    <definedName name="_xlchart.v1.12" hidden="1">Sheet1!$C$70:$C$119</definedName>
-    <definedName name="_xlchart.v1.13" hidden="1">Sheet1!$A$2:$A$51</definedName>
-    <definedName name="_xlchart.v1.14" hidden="1">Sheet1!$F$1</definedName>
-    <definedName name="_xlchart.v1.15" hidden="1">Sheet1!$F$2:$F$51</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">Sheet1!$B$1</definedName>
+    <definedName name="_xlchart.v1.10" hidden="1">Sheet1!$O$2:$O$51</definedName>
+    <definedName name="_xlchart.v1.11" hidden="1">Sheet1!$A$71:$A$120</definedName>
+    <definedName name="_xlchart.v1.12" hidden="1">Sheet1!$B$70</definedName>
+    <definedName name="_xlchart.v1.13" hidden="1">Sheet1!$B$71:$B$120</definedName>
+    <definedName name="_xlchart.v1.14" hidden="1">Sheet1!$C$70</definedName>
+    <definedName name="_xlchart.v1.15" hidden="1">Sheet1!$C$71:$C$120</definedName>
     <definedName name="_xlchart.v1.16" hidden="1">Sheet1!$A$2:$A$51</definedName>
-    <definedName name="_xlchart.v1.17" hidden="1">Sheet1!$H$1</definedName>
-    <definedName name="_xlchart.v1.18" hidden="1">Sheet1!$H$2:$H$51</definedName>
+    <definedName name="_xlchart.v1.17" hidden="1">Sheet1!$L$1</definedName>
+    <definedName name="_xlchart.v1.18" hidden="1">Sheet1!$L$2:$L$51</definedName>
     <definedName name="_xlchart.v1.19" hidden="1">Sheet1!$A$2:$A$51</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">Sheet1!$L$2:$L$51</definedName>
-    <definedName name="_xlchart.v1.20" hidden="1">Sheet1!$O$1</definedName>
-    <definedName name="_xlchart.v1.21" hidden="1">Sheet1!$O$2:$O$51</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">Sheet1!$A$2:$A$51</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">Sheet1!$B$1</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">Sheet1!$B$2:$B$51</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">Sheet1!$C$1</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">Sheet1!$C$2:$C$51</definedName>
-    <definedName name="_xlchart.v1.8" hidden="1">Sheet1!$A$70:$A$119</definedName>
-    <definedName name="_xlchart.v1.9" hidden="1">Sheet1!$B$69</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">Sheet1!$B$2:$B$51</definedName>
+    <definedName name="_xlchart.v1.20" hidden="1">Sheet1!$F$1</definedName>
+    <definedName name="_xlchart.v1.21" hidden="1">Sheet1!$F$2:$F$51</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">Sheet1!$C$1</definedName>
+    <definedName name="_xlchart.v1.4" hidden="1">Sheet1!$C$2:$C$51</definedName>
+    <definedName name="_xlchart.v1.5" hidden="1">Sheet1!$A$2:$A$51</definedName>
+    <definedName name="_xlchart.v1.6" hidden="1">Sheet1!$H$1</definedName>
+    <definedName name="_xlchart.v1.7" hidden="1">Sheet1!$H$2:$H$51</definedName>
+    <definedName name="_xlchart.v1.8" hidden="1">Sheet1!$A$2:$A$51</definedName>
+    <definedName name="_xlchart.v1.9" hidden="1">Sheet1!$O$1</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="102">
   <si>
     <t>State</t>
   </si>
@@ -354,6 +354,9 @@
   <si>
     <t>State Motor Fuel Tax  - on producers (decimal)</t>
   </si>
+  <si>
+    <t>MEDIAN</t>
+  </si>
 </sst>
 </file>
 
@@ -469,7 +472,7 @@
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -506,6 +509,12 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Calculation" xfId="2" builtinId="22"/>
@@ -4474,18 +4483,18 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:strDim type="cat">
-        <cx:f>_xlchart.v1.3</cx:f>
+        <cx:f>_xlchart.v1.0</cx:f>
       </cx:strDim>
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.5</cx:f>
+        <cx:f>_xlchart.v1.2</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="1">
       <cx:strDim type="cat">
-        <cx:f>_xlchart.v1.3</cx:f>
+        <cx:f>_xlchart.v1.0</cx:f>
       </cx:strDim>
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.7</cx:f>
+        <cx:f>_xlchart.v1.4</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -4523,7 +4532,7 @@
         <cx:series layoutId="clusteredColumn" hidden="1" uniqueId="{FC2F3EC4-C96E-3340-87B8-70D66843A149}" formatIdx="0">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.4</cx:f>
+              <cx:f>_xlchart.v1.1</cx:f>
               <cx:v/>
             </cx:txData>
           </cx:tx>
@@ -4535,7 +4544,7 @@
         <cx:series layoutId="clusteredColumn" uniqueId="{BDA3C212-6CA2-2840-BB48-235B6854C402}" formatIdx="1">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.6</cx:f>
+              <cx:f>_xlchart.v1.3</cx:f>
               <cx:v>Income Tax Rate (decimal)</cx:v>
             </cx:txData>
           </cx:tx>
@@ -4566,18 +4575,18 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:strDim type="cat">
-        <cx:f>_xlchart.v1.8</cx:f>
+        <cx:f>_xlchart.v1.11</cx:f>
       </cx:strDim>
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.10</cx:f>
+        <cx:f>_xlchart.v1.13</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="1">
       <cx:strDim type="cat">
-        <cx:f>_xlchart.v1.8</cx:f>
+        <cx:f>_xlchart.v1.11</cx:f>
       </cx:strDim>
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.12</cx:f>
+        <cx:f>_xlchart.v1.15</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -4587,7 +4596,7 @@
         <cx:series layoutId="clusteredColumn" hidden="1" uniqueId="{DB5E0DEC-BDD7-E045-B50E-E9E5077B84A0}" formatIdx="0">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.9</cx:f>
+              <cx:f>_xlchart.v1.12</cx:f>
               <cx:v/>
             </cx:txData>
           </cx:tx>
@@ -4599,7 +4608,7 @@
         <cx:series layoutId="clusteredColumn" uniqueId="{534AC433-1553-B047-BF3B-BCE89F08CC46}" formatIdx="1">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.11</cx:f>
+              <cx:f>_xlchart.v1.14</cx:f>
               <cx:v>Electricity Price (USD/kWh)</cx:v>
             </cx:txData>
           </cx:tx>
@@ -4630,10 +4639,10 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:strDim type="cat">
-        <cx:f>_xlchart.v1.13</cx:f>
+        <cx:f>_xlchart.v1.19</cx:f>
       </cx:strDim>
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.15</cx:f>
+        <cx:f>_xlchart.v1.21</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -4671,7 +4680,7 @@
         <cx:series layoutId="clusteredColumn" uniqueId="{9CC3CEB9-8BC1-0D4B-9E6A-350019E85A1C}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.14</cx:f>
+              <cx:f>_xlchart.v1.20</cx:f>
               <cx:v>Property Tax Rate (decimal)</cx:v>
             </cx:txData>
           </cx:tx>
@@ -4702,10 +4711,10 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:strDim type="cat">
-        <cx:f>_xlchart.v1.16</cx:f>
+        <cx:f>_xlchart.v1.5</cx:f>
       </cx:strDim>
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.18</cx:f>
+        <cx:f>_xlchart.v1.7</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -4743,7 +4752,7 @@
         <cx:series layoutId="clusteredColumn" uniqueId="{841AD1B4-5AC3-6746-BCB8-C3142F68F518}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.17</cx:f>
+              <cx:f>_xlchart.v1.6</cx:f>
               <cx:v>State Motor Fuel Tax  - at pump (USD/gal)</cx:v>
             </cx:txData>
           </cx:tx>
@@ -4774,10 +4783,10 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:strDim type="cat">
-        <cx:f>_xlchart.v1.0</cx:f>
+        <cx:f>_xlchart.v1.16</cx:f>
       </cx:strDim>
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.2</cx:f>
+        <cx:f>_xlchart.v1.18</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -4815,7 +4824,7 @@
         <cx:series layoutId="clusteredColumn" uniqueId="{00D4F7D1-BF74-0E44-ACE4-63518A652FA3}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.1</cx:f>
+              <cx:f>_xlchart.v1.17</cx:f>
               <cx:v>Sales Tax Rate (decimal)</cx:v>
             </cx:txData>
           </cx:tx>
@@ -4846,10 +4855,10 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:strDim type="cat">
-        <cx:f>_xlchart.v1.19</cx:f>
+        <cx:f>_xlchart.v1.8</cx:f>
       </cx:strDim>
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.21</cx:f>
+        <cx:f>_xlchart.v1.10</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -4887,7 +4896,7 @@
         <cx:series layoutId="clusteredColumn" uniqueId="{8ED5D8B4-47C5-E641-AE5A-567D89B76F43}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.20</cx:f>
+              <cx:f>_xlchart.v1.9</cx:f>
               <cx:v>Location Capital Cost Factor (unitless)</cx:v>
             </cx:txData>
           </cx:tx>
@@ -11655,13 +11664,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>209550</xdr:colOff>
-      <xdr:row>53</xdr:row>
+      <xdr:row>54</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>654050</xdr:colOff>
-      <xdr:row>67</xdr:row>
+      <xdr:row>68</xdr:row>
       <xdr:rowOff>139700</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -11739,7 +11748,7 @@
     <xdr:to>
       <xdr:col>26</xdr:col>
       <xdr:colOff>444500</xdr:colOff>
-      <xdr:row>59</xdr:row>
+      <xdr:row>60</xdr:row>
       <xdr:rowOff>101600</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -11771,13 +11780,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>139700</xdr:colOff>
-      <xdr:row>69</xdr:row>
+      <xdr:row>70</xdr:row>
       <xdr:rowOff>82550</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>285750</xdr:colOff>
-      <xdr:row>82</xdr:row>
+      <xdr:row>83</xdr:row>
       <xdr:rowOff>184150</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -11887,13 +11896,13 @@
     <xdr:from>
       <xdr:col>9</xdr:col>
       <xdr:colOff>615950</xdr:colOff>
-      <xdr:row>53</xdr:row>
+      <xdr:row>54</xdr:row>
       <xdr:rowOff>127000</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
       <xdr:colOff>234950</xdr:colOff>
-      <xdr:row>67</xdr:row>
+      <xdr:row>68</xdr:row>
       <xdr:rowOff>25400</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -11965,13 +11974,13 @@
     <xdr:from>
       <xdr:col>9</xdr:col>
       <xdr:colOff>527050</xdr:colOff>
-      <xdr:row>69</xdr:row>
+      <xdr:row>70</xdr:row>
       <xdr:rowOff>63500</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
       <xdr:colOff>146050</xdr:colOff>
-      <xdr:row>82</xdr:row>
+      <xdr:row>83</xdr:row>
       <xdr:rowOff>165100</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -12043,13 +12052,13 @@
     <xdr:from>
       <xdr:col>9</xdr:col>
       <xdr:colOff>457200</xdr:colOff>
-      <xdr:row>83</xdr:row>
+      <xdr:row>84</xdr:row>
       <xdr:rowOff>101600</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
       <xdr:colOff>76200</xdr:colOff>
-      <xdr:row>98</xdr:row>
+      <xdr:row>99</xdr:row>
       <xdr:rowOff>12700</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -12121,13 +12130,13 @@
     <xdr:from>
       <xdr:col>9</xdr:col>
       <xdr:colOff>431800</xdr:colOff>
-      <xdr:row>98</xdr:row>
+      <xdr:row>99</xdr:row>
       <xdr:rowOff>88900</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
       <xdr:colOff>50800</xdr:colOff>
-      <xdr:row>111</xdr:row>
+      <xdr:row>112</xdr:row>
       <xdr:rowOff>190500</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -12536,10 +12545,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CC2A6F1-FF40-DF41-A5E2-6E4FBD4236BC}">
-  <dimension ref="A1:R119"/>
+  <dimension ref="A1:R120"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2:L51"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -15165,479 +15174,526 @@
       </c>
     </row>
     <row r="53" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="M53" s="4"/>
+      <c r="A53" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B53" s="1"/>
+      <c r="C53" s="18">
+        <f>_xlfn.PERCENTILE.INC(C2:C51,0.5)</f>
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="D53" s="18">
+        <f t="shared" ref="D53:P53" si="4">_xlfn.PERCENTILE.INC(D2:D51,0.5)</f>
+        <v>0.87</v>
+      </c>
+      <c r="E53" s="18">
+        <f t="shared" si="4"/>
+        <v>1.3</v>
+      </c>
+      <c r="F53" s="19">
+        <f t="shared" si="4"/>
+        <v>1.3559499999999999E-2</v>
+      </c>
+      <c r="G53" s="18"/>
+      <c r="H53" s="18"/>
+      <c r="I53" s="18"/>
+      <c r="J53" s="18"/>
+      <c r="K53" s="18">
+        <f t="shared" si="4"/>
+        <v>5.875</v>
+      </c>
+      <c r="L53" s="18">
+        <f t="shared" si="4"/>
+        <v>5.8749999999999997E-2</v>
+      </c>
+      <c r="M53" s="19">
+        <f t="shared" si="4"/>
+        <v>6.8500000000000005E-2</v>
+      </c>
+      <c r="N53" s="18"/>
+      <c r="O53" s="16">
+        <f t="shared" si="4"/>
+        <v>1.0231576439191701</v>
+      </c>
+      <c r="P53" s="16">
+        <f t="shared" si="4"/>
+        <v>0.50515179999999993</v>
+      </c>
     </row>
     <row r="54" spans="1:18" x14ac:dyDescent="0.2">
       <c r="M54" s="4"/>
     </row>
     <row r="55" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="L55" s="4"/>
+      <c r="M55" s="4"/>
     </row>
     <row r="56" spans="1:18" x14ac:dyDescent="0.2">
       <c r="L56" s="4"/>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A69" s="1" t="s">
+    <row r="57" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="L57" s="4"/>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A70" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C69" s="1" t="s">
+      <c r="C70" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="D69" s="1"/>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A70" t="s">
-        <v>2</v>
-      </c>
-      <c r="C70" s="4">
-        <v>6.0100000000000001E-2</v>
-      </c>
-      <c r="D70" s="4"/>
+      <c r="D70" s="1"/>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C71" s="4">
-        <v>0.17100000000000001</v>
+        <v>6.0100000000000001E-2</v>
       </c>
       <c r="D71" s="4"/>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C72" s="4">
-        <v>6.5500000000000003E-2</v>
+        <v>0.17100000000000001</v>
       </c>
       <c r="D72" s="4"/>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C73" s="4">
-        <v>5.6399999999999999E-2</v>
+        <v>6.5500000000000003E-2</v>
       </c>
       <c r="D73" s="4"/>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C74" s="4">
-        <v>0.13200000000000001</v>
+        <v>5.6399999999999999E-2</v>
       </c>
       <c r="D74" s="4"/>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C75" s="4">
-        <v>7.4700000000000003E-2</v>
+        <v>0.13200000000000001</v>
       </c>
       <c r="D75" s="4"/>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C76" s="4">
-        <v>0.13769999999999999</v>
+        <v>7.4700000000000003E-2</v>
       </c>
       <c r="D76" s="4"/>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C77" s="4">
-        <v>7.9500000000000001E-2</v>
+        <v>0.13769999999999999</v>
       </c>
       <c r="D77" s="4"/>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C78" s="4">
-        <v>7.6499999999999999E-2</v>
+        <v>7.9500000000000001E-2</v>
       </c>
       <c r="D78" s="4"/>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C79" s="4">
-        <v>0.06</v>
+        <v>7.6499999999999999E-2</v>
       </c>
       <c r="D79" s="4"/>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C80" s="4">
-        <v>0.26100000000000001</v>
+        <v>0.06</v>
       </c>
       <c r="D80" s="4"/>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C81" s="4">
-        <v>6.4699999999999994E-2</v>
+        <v>0.26100000000000001</v>
       </c>
       <c r="D81" s="4"/>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C82" s="4">
-        <v>6.8000000000000005E-2</v>
+        <v>6.4699999999999994E-2</v>
       </c>
       <c r="D82" s="4"/>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C83" s="4">
-        <v>7.3800000000000004E-2</v>
+        <v>6.8000000000000005E-2</v>
       </c>
       <c r="D83" s="4"/>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C84" s="4">
-        <v>6.4500000000000002E-2</v>
+        <v>7.3800000000000004E-2</v>
       </c>
       <c r="D84" s="4"/>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C85" s="4">
-        <v>7.5999999999999998E-2</v>
+        <v>6.4500000000000002E-2</v>
       </c>
       <c r="D85" s="4"/>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C86" s="4">
-        <v>5.6800000000000003E-2</v>
+        <v>7.5999999999999998E-2</v>
       </c>
       <c r="D86" s="4"/>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C87" s="4">
-        <v>5.3499999999999999E-2</v>
+        <v>5.6800000000000003E-2</v>
       </c>
       <c r="D87" s="4"/>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C88" s="4">
-        <v>9.3200000000000005E-2</v>
+        <v>5.3499999999999999E-2</v>
       </c>
       <c r="D88" s="4"/>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C89" s="4">
-        <v>8.2299999999999998E-2</v>
+        <v>9.3200000000000005E-2</v>
       </c>
       <c r="D89" s="4"/>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C90" s="4">
-        <v>0.1489</v>
+        <v>8.2299999999999998E-2</v>
       </c>
       <c r="D90" s="4"/>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C91" s="4">
-        <v>7.0999999999999994E-2</v>
+        <v>0.1489</v>
       </c>
       <c r="D91" s="4"/>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C92" s="4">
-        <v>7.5200000000000003E-2</v>
+        <v>7.0999999999999994E-2</v>
       </c>
       <c r="D92" s="4"/>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>52</v>
+        <v>25</v>
       </c>
       <c r="C93" s="4">
-        <v>0.06</v>
+        <v>7.5200000000000003E-2</v>
       </c>
       <c r="D93" s="4"/>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>26</v>
+        <v>52</v>
       </c>
       <c r="C94" s="4">
-        <v>7.22E-2</v>
+        <v>0.06</v>
       </c>
       <c r="D94" s="4"/>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C95" s="4">
-        <v>5.1900000000000002E-2</v>
+        <v>7.22E-2</v>
       </c>
       <c r="D95" s="4"/>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C96" s="4">
-        <v>7.5999999999999998E-2</v>
+        <v>5.1900000000000002E-2</v>
       </c>
       <c r="D96" s="4"/>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C97" s="4">
-        <v>6.0999999999999999E-2</v>
+        <v>7.5999999999999998E-2</v>
       </c>
       <c r="D97" s="4"/>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C98" s="4">
-        <v>0.13420000000000001</v>
+        <v>6.0999999999999999E-2</v>
       </c>
       <c r="D98" s="4"/>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C99" s="4">
-        <v>0.1007</v>
+        <v>0.13420000000000001</v>
       </c>
       <c r="D99" s="4"/>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C100" s="4">
-        <v>5.8400000000000001E-2</v>
+        <v>0.1007</v>
       </c>
       <c r="D100" s="4"/>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C101" s="4">
-        <v>6.0199999999999997E-2</v>
+        <v>5.8400000000000001E-2</v>
       </c>
       <c r="D101" s="4"/>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C102" s="4">
-        <v>6.3299999999999995E-2</v>
+        <v>6.0199999999999997E-2</v>
       </c>
       <c r="D102" s="4"/>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C103" s="4">
-        <v>7.9799999999999996E-2</v>
+        <v>6.3299999999999995E-2</v>
       </c>
       <c r="D103" s="4"/>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C104" s="4">
-        <v>7.0099999999999996E-2</v>
+        <v>7.9799999999999996E-2</v>
       </c>
       <c r="D104" s="4"/>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C105" s="4">
-        <v>5.3400000000000003E-2</v>
+        <v>7.0099999999999996E-2</v>
       </c>
       <c r="D105" s="4"/>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C106" s="4">
-        <v>5.8599999999999999E-2</v>
+        <v>5.3400000000000003E-2</v>
       </c>
       <c r="D106" s="4"/>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C107" s="4">
-        <v>6.8400000000000002E-2</v>
+        <v>5.8599999999999999E-2</v>
       </c>
       <c r="D107" s="4"/>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>40</v>
-      </c>
-      <c r="C108" s="8">
-        <v>0.15390000000000001</v>
-      </c>
-      <c r="D108" s="8"/>
+        <v>39</v>
+      </c>
+      <c r="C108" s="4">
+        <v>6.8400000000000002E-2</v>
+      </c>
+      <c r="D108" s="4"/>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C109" s="8">
-        <v>6.0999999999999999E-2</v>
+        <v>0.15390000000000001</v>
       </c>
       <c r="D109" s="8"/>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C110" s="8">
-        <v>7.7700000000000005E-2</v>
+        <v>6.0999999999999999E-2</v>
       </c>
       <c r="D110" s="8"/>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>43</v>
-      </c>
-      <c r="C111" s="4">
-        <v>5.6800000000000003E-2</v>
-      </c>
-      <c r="D111" s="4"/>
+        <v>42</v>
+      </c>
+      <c r="C111" s="8">
+        <v>7.7700000000000005E-2</v>
+      </c>
+      <c r="D111" s="8"/>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C112" s="4">
-        <v>5.3900000000000003E-2</v>
+        <v>5.6800000000000003E-2</v>
       </c>
       <c r="D112" s="4"/>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C113" s="4">
-        <v>5.8999999999999997E-2</v>
+        <v>5.3900000000000003E-2</v>
       </c>
       <c r="D113" s="4"/>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C114" s="4">
-        <v>0.1066</v>
+        <v>5.8999999999999997E-2</v>
       </c>
       <c r="D114" s="4"/>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C115" s="4">
-        <v>6.8599999999999994E-2</v>
+        <v>0.1066</v>
       </c>
       <c r="D115" s="4"/>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C116" s="4">
-        <v>4.7100000000000003E-2</v>
+        <v>6.8599999999999994E-2</v>
       </c>
       <c r="D116" s="4"/>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C117" s="4">
-        <v>6.4000000000000001E-2</v>
+        <v>4.7100000000000003E-2</v>
       </c>
       <c r="D117" s="4"/>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C118" s="4">
-        <v>7.3300000000000004E-2</v>
+        <v>6.4000000000000001E-2</v>
       </c>
       <c r="D118" s="4"/>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
+        <v>50</v>
+      </c>
+      <c r="C119" s="4">
+        <v>7.3300000000000004E-2</v>
+      </c>
+      <c r="D119" s="4"/>
+    </row>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A120" t="s">
         <v>51</v>
       </c>
-      <c r="C119" s="4">
+      <c r="C120" s="4">
         <v>6.7100000000000007E-2</v>
       </c>
-      <c r="D119" s="4"/>
+      <c r="D120" s="4"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="N59:O109">
-    <sortCondition ref="N59:N109"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="N60:O110">
+    <sortCondition ref="N60:N110"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
almost final updates to all files
</commit_message>
<xml_diff>
--- a/incentives/state_specific_data.xlsx
+++ b/incentives/state_specific_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daltonstewart/Dropbox/Stewart-Guest_Shared/Code/Biorefinery-Tax-Incentives/incentives/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5C925D7-9CA1-EA48-876E-EA773A86CE8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FF6DB7E-D63E-E548-B393-11A42CB51D4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15800" xr2:uid="{ACA89B21-CD83-0545-80CD-93A328B5FE1A}"/>
   </bookViews>
@@ -18,27 +18,27 @@
   </sheets>
   <definedNames>
     <definedName name="_xlchart.v1.0" hidden="1">Sheet1!$A$2:$A$51</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">Sheet1!$B$1</definedName>
-    <definedName name="_xlchart.v1.10" hidden="1">Sheet1!$O$2:$O$51</definedName>
-    <definedName name="_xlchart.v1.11" hidden="1">Sheet1!$A$71:$A$120</definedName>
-    <definedName name="_xlchart.v1.12" hidden="1">Sheet1!$B$70</definedName>
-    <definedName name="_xlchart.v1.13" hidden="1">Sheet1!$B$71:$B$120</definedName>
-    <definedName name="_xlchart.v1.14" hidden="1">Sheet1!$C$70</definedName>
-    <definedName name="_xlchart.v1.15" hidden="1">Sheet1!$C$71:$C$120</definedName>
-    <definedName name="_xlchart.v1.16" hidden="1">Sheet1!$A$2:$A$51</definedName>
-    <definedName name="_xlchart.v1.17" hidden="1">Sheet1!$L$1</definedName>
-    <definedName name="_xlchart.v1.18" hidden="1">Sheet1!$L$2:$L$51</definedName>
-    <definedName name="_xlchart.v1.19" hidden="1">Sheet1!$A$2:$A$51</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">Sheet1!$B$2:$B$51</definedName>
-    <definedName name="_xlchart.v1.20" hidden="1">Sheet1!$F$1</definedName>
-    <definedName name="_xlchart.v1.21" hidden="1">Sheet1!$F$2:$F$51</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">Sheet1!$C$1</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">Sheet1!$C$2:$C$51</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">Sheet1!$A$2:$A$51</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">Sheet1!$H$1</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">Sheet1!$H$2:$H$51</definedName>
-    <definedName name="_xlchart.v1.8" hidden="1">Sheet1!$A$2:$A$51</definedName>
-    <definedName name="_xlchart.v1.9" hidden="1">Sheet1!$O$1</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">Sheet1!$L$1</definedName>
+    <definedName name="_xlchart.v1.10" hidden="1">Sheet1!$H$1</definedName>
+    <definedName name="_xlchart.v1.11" hidden="1">Sheet1!$H$2:$H$51</definedName>
+    <definedName name="_xlchart.v1.12" hidden="1">Sheet1!$A$71:$A$120</definedName>
+    <definedName name="_xlchart.v1.13" hidden="1">Sheet1!$B$70</definedName>
+    <definedName name="_xlchart.v1.14" hidden="1">Sheet1!$B$71:$B$120</definedName>
+    <definedName name="_xlchart.v1.15" hidden="1">Sheet1!$C$70</definedName>
+    <definedName name="_xlchart.v1.16" hidden="1">Sheet1!$C$71:$C$120</definedName>
+    <definedName name="_xlchart.v1.17" hidden="1">Sheet1!$A$2:$A$51</definedName>
+    <definedName name="_xlchart.v1.18" hidden="1">Sheet1!$B$1</definedName>
+    <definedName name="_xlchart.v1.19" hidden="1">Sheet1!$B$2:$B$51</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">Sheet1!$L$2:$L$51</definedName>
+    <definedName name="_xlchart.v1.20" hidden="1">Sheet1!$C$1</definedName>
+    <definedName name="_xlchart.v1.21" hidden="1">Sheet1!$C$2:$C$51</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">Sheet1!$A$2:$A$51</definedName>
+    <definedName name="_xlchart.v1.4" hidden="1">Sheet1!$O$1</definedName>
+    <definedName name="_xlchart.v1.5" hidden="1">Sheet1!$O$2:$O$51</definedName>
+    <definedName name="_xlchart.v1.6" hidden="1">Sheet1!$A$2:$A$51</definedName>
+    <definedName name="_xlchart.v1.7" hidden="1">Sheet1!$F$1</definedName>
+    <definedName name="_xlchart.v1.8" hidden="1">Sheet1!$F$2:$F$51</definedName>
+    <definedName name="_xlchart.v1.9" hidden="1">Sheet1!$A$2:$A$51</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -4483,18 +4483,18 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:strDim type="cat">
-        <cx:f>_xlchart.v1.0</cx:f>
+        <cx:f>_xlchart.v1.17</cx:f>
       </cx:strDim>
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.2</cx:f>
+        <cx:f>_xlchart.v1.19</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="1">
       <cx:strDim type="cat">
-        <cx:f>_xlchart.v1.0</cx:f>
+        <cx:f>_xlchart.v1.17</cx:f>
       </cx:strDim>
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.4</cx:f>
+        <cx:f>_xlchart.v1.21</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -4532,7 +4532,7 @@
         <cx:series layoutId="clusteredColumn" hidden="1" uniqueId="{FC2F3EC4-C96E-3340-87B8-70D66843A149}" formatIdx="0">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.1</cx:f>
+              <cx:f>_xlchart.v1.18</cx:f>
               <cx:v/>
             </cx:txData>
           </cx:tx>
@@ -4544,7 +4544,7 @@
         <cx:series layoutId="clusteredColumn" uniqueId="{BDA3C212-6CA2-2840-BB48-235B6854C402}" formatIdx="1">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.3</cx:f>
+              <cx:f>_xlchart.v1.20</cx:f>
               <cx:v>Income Tax Rate (decimal)</cx:v>
             </cx:txData>
           </cx:tx>
@@ -4575,18 +4575,18 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:strDim type="cat">
-        <cx:f>_xlchart.v1.11</cx:f>
+        <cx:f>_xlchart.v1.12</cx:f>
       </cx:strDim>
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.13</cx:f>
+        <cx:f>_xlchart.v1.14</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="1">
       <cx:strDim type="cat">
-        <cx:f>_xlchart.v1.11</cx:f>
+        <cx:f>_xlchart.v1.12</cx:f>
       </cx:strDim>
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.15</cx:f>
+        <cx:f>_xlchart.v1.16</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -4596,7 +4596,7 @@
         <cx:series layoutId="clusteredColumn" hidden="1" uniqueId="{DB5E0DEC-BDD7-E045-B50E-E9E5077B84A0}" formatIdx="0">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.12</cx:f>
+              <cx:f>_xlchart.v1.13</cx:f>
               <cx:v/>
             </cx:txData>
           </cx:tx>
@@ -4608,7 +4608,7 @@
         <cx:series layoutId="clusteredColumn" uniqueId="{534AC433-1553-B047-BF3B-BCE89F08CC46}" formatIdx="1">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.14</cx:f>
+              <cx:f>_xlchart.v1.15</cx:f>
               <cx:v>Electricity Price (USD/kWh)</cx:v>
             </cx:txData>
           </cx:tx>
@@ -4639,10 +4639,10 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:strDim type="cat">
-        <cx:f>_xlchart.v1.19</cx:f>
+        <cx:f>_xlchart.v1.6</cx:f>
       </cx:strDim>
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.21</cx:f>
+        <cx:f>_xlchart.v1.8</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -4680,7 +4680,7 @@
         <cx:series layoutId="clusteredColumn" uniqueId="{9CC3CEB9-8BC1-0D4B-9E6A-350019E85A1C}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.20</cx:f>
+              <cx:f>_xlchart.v1.7</cx:f>
               <cx:v>Property Tax Rate (decimal)</cx:v>
             </cx:txData>
           </cx:tx>
@@ -4711,10 +4711,10 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:strDim type="cat">
-        <cx:f>_xlchart.v1.5</cx:f>
+        <cx:f>_xlchart.v1.9</cx:f>
       </cx:strDim>
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.7</cx:f>
+        <cx:f>_xlchart.v1.11</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -4752,7 +4752,7 @@
         <cx:series layoutId="clusteredColumn" uniqueId="{841AD1B4-5AC3-6746-BCB8-C3142F68F518}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.6</cx:f>
+              <cx:f>_xlchart.v1.10</cx:f>
               <cx:v>State Motor Fuel Tax  - at pump (USD/gal)</cx:v>
             </cx:txData>
           </cx:tx>
@@ -4783,10 +4783,10 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:strDim type="cat">
-        <cx:f>_xlchart.v1.16</cx:f>
+        <cx:f>_xlchart.v1.0</cx:f>
       </cx:strDim>
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.18</cx:f>
+        <cx:f>_xlchart.v1.2</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -4824,7 +4824,7 @@
         <cx:series layoutId="clusteredColumn" uniqueId="{00D4F7D1-BF74-0E44-ACE4-63518A652FA3}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.17</cx:f>
+              <cx:f>_xlchart.v1.1</cx:f>
               <cx:v>Sales Tax Rate (decimal)</cx:v>
             </cx:txData>
           </cx:tx>
@@ -4855,10 +4855,10 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:strDim type="cat">
-        <cx:f>_xlchart.v1.8</cx:f>
+        <cx:f>_xlchart.v1.3</cx:f>
       </cx:strDim>
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.10</cx:f>
+        <cx:f>_xlchart.v1.5</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -4896,7 +4896,7 @@
         <cx:series layoutId="clusteredColumn" uniqueId="{8ED5D8B4-47C5-E641-AE5A-567D89B76F43}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.9</cx:f>
+              <cx:f>_xlchart.v1.4</cx:f>
               <cx:v>Location Capital Cost Factor (unitless)</cx:v>
             </cx:txData>
           </cx:tx>
@@ -11707,7 +11707,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="209550" y="10807700"/>
+              <a:off x="209550" y="11010900"/>
               <a:ext cx="4572000" cy="2946400"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -11823,7 +11823,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="139700" y="14103350"/>
+              <a:off x="139700" y="14306550"/>
               <a:ext cx="4273550" cy="2743200"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -11939,7 +11939,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="5568950" y="10896600"/>
+              <a:off x="5568950" y="11099800"/>
               <a:ext cx="5397500" cy="2743200"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -12017,7 +12017,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="5480050" y="14084300"/>
+              <a:off x="5480050" y="14287500"/>
               <a:ext cx="5397500" cy="2743200"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -12095,7 +12095,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="5410200" y="16967200"/>
+              <a:off x="5410200" y="17170400"/>
               <a:ext cx="5397500" cy="2959100"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -12173,7 +12173,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="5384800" y="20002500"/>
+              <a:off x="5384800" y="20205700"/>
               <a:ext cx="5397500" cy="2743200"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -12548,7 +12548,7 @@
   <dimension ref="A1:R120"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="A2" sqref="A2:A51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>